<commit_message>
add rasd analysis, begin ramal al-maya
</commit_message>
<xml_diff>
--- a/Analysis/motive charts/chromatic motives.xlsx
+++ b/Analysis/motive charts/chromatic motives.xlsx
@@ -1960,11 +1960,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2117264680"/>
-        <c:axId val="2141459080"/>
+        <c:axId val="-2132263576"/>
+        <c:axId val="-2132260456"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2117264680"/>
+        <c:axId val="-2132263576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1974,7 +1974,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141459080"/>
+        <c:crossAx val="-2132260456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1982,7 +1982,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141459080"/>
+        <c:axId val="-2132260456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1993,7 +1993,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117264680"/>
+        <c:crossAx val="-2132263576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3473,11 +3473,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2114556216"/>
-        <c:axId val="-2115124424"/>
+        <c:axId val="-2132013576"/>
+        <c:axId val="-2131812248"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2114556216"/>
+        <c:axId val="-2132013576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3487,7 +3487,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115124424"/>
+        <c:crossAx val="-2131812248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3495,7 +3495,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115124424"/>
+        <c:axId val="-2131812248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3506,7 +3506,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114556216"/>
+        <c:crossAx val="-2132013576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3563,15 +3563,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3919,7 +3919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DF80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
       <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>

</xml_diff>